<commit_message>
plotted phylum level t8 lca
</commit_message>
<xml_diff>
--- a/analyses/T8-notincs/unipept/lca/NAAF/BY_GF75_675_676_sorting.xlsx
+++ b/analyses/T8-notincs/unipept/lca/NAAF/BY_GF75_675_676_sorting.xlsx
@@ -573,7 +573,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.91"/>
@@ -587,7 +587,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.52"/>
@@ -1227,10 +1227,10 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.35"/>
@@ -1532,11 +1532,11 @@
   </sheetPr>
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1578,6 +1578,9 @@
       <c r="B4" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -1597,6 +1600,9 @@
       <c r="B6" s="0" t="n">
         <v>6.82878465348421</v>
       </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -1605,6 +1611,9 @@
       <c r="B7" s="0" t="n">
         <v>6.82878465348421</v>
       </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -1613,6 +1622,9 @@
       <c r="B8" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -1621,6 +1633,9 @@
       <c r="B9" s="0" t="n">
         <v>6.82878465348421</v>
       </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -1629,6 +1644,9 @@
       <c r="B10" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -1637,6 +1655,9 @@
       <c r="B11" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -1645,6 +1666,9 @@
       <c r="B12" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C12" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -1653,6 +1677,9 @@
       <c r="B13" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -1661,6 +1688,9 @@
       <c r="B14" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C14" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -1669,6 +1699,9 @@
       <c r="B15" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C15" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -1677,6 +1710,9 @@
       <c r="B16" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -1685,6 +1721,9 @@
       <c r="B17" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C17" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -1693,6 +1732,9 @@
       <c r="B18" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -1701,6 +1743,9 @@
       <c r="B19" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C19" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -1709,6 +1754,9 @@
       <c r="B20" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C20" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -1717,6 +1765,9 @@
       <c r="B21" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C21" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -1725,6 +1776,9 @@
       <c r="B22" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C22" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -1744,6 +1798,9 @@
       <c r="B24" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C24" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
@@ -1752,6 +1809,9 @@
       <c r="B25" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C25" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -1760,6 +1820,9 @@
       <c r="B26" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C26" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
@@ -1768,6 +1831,9 @@
       <c r="B27" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C27" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -1776,6 +1842,9 @@
       <c r="B28" s="0" t="n">
         <v>0.0999575724640442</v>
       </c>
+      <c r="C28" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -1784,6 +1853,9 @@
       <c r="B29" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C29" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -1792,6 +1864,9 @@
       <c r="B30" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C30" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
@@ -1800,6 +1875,9 @@
       <c r="B31" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C31" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -1808,6 +1886,9 @@
       <c r="B32" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C32" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
@@ -1816,6 +1897,9 @@
       <c r="B33" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C33" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
@@ -1824,6 +1908,9 @@
       <c r="B34" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C34" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
@@ -1832,6 +1919,9 @@
       <c r="B35" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C35" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
@@ -1840,6 +1930,9 @@
       <c r="B36" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C36" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
@@ -1848,12 +1941,18 @@
       <c r="B37" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="C37" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>134</v>
       </c>
       <c r="B38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1879,7 +1978,7 @@
       <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.13"/>
@@ -1898,10 +1997,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="12.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="22.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="15.74"/>
@@ -2425,7 +2524,7 @@
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.35"/>

</xml_diff>